<commit_message>
Shifted general write functions to write_tome_lowlevel. Added general write_tome_vector().
</commit_message>
<xml_diff>
--- a/tome_cheatsheet.xlsx
+++ b/tome_cheatsheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17625"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="12750"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="80">
   <si>
     <t>exon/</t>
   </si>
@@ -259,13 +259,19 @@
   </si>
   <si>
     <t>/</t>
+  </si>
+  <si>
+    <t>read_tome_projection()</t>
+  </si>
+  <si>
+    <t>read_tome_projection_desc()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -309,6 +315,11 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -330,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -350,6 +361,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1062,15 +1074,17 @@
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="C40" s="2"/>
       <c r="F40" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C41" s="4" t="s">
+      <c r="B41" s="2"/>
+      <c r="C41" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F41" t="s">
@@ -1079,12 +1093,13 @@
       <c r="G41" t="s">
         <v>42</v>
       </c>
-      <c r="H41" s="8" t="s">
-        <v>41</v>
+      <c r="H41" s="9" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C42" s="4" t="s">
+      <c r="B42" s="2"/>
+      <c r="C42" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F42" t="s">
@@ -1093,8 +1108,8 @@
       <c r="G42" t="s">
         <v>43</v>
       </c>
-      <c r="H42" s="8" t="s">
-        <v>41</v>
+      <c r="H42" s="9" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.2">

</xml_diff>